<commit_message>
Fixed-All columns returned After Z
</commit_message>
<xml_diff>
--- a/items1.xlsx
+++ b/items1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SURESH GARG\Desktop\webdev\multiply3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3638EAF1-24D0-4E34-9084-B1345F0F0886}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D42C99C-67C3-48D8-A84F-500A82FE7824}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{13DD2B88-E29A-446D-86D8-2EDDC9A8D7C9}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="110">
   <si>
     <t>schemaVersion</t>
   </si>
@@ -356,6 +356,15 @@
   </si>
   <si>
     <t>aud</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>bb</t>
+  </si>
+  <si>
+    <t>bbb</t>
   </si>
 </sst>
 </file>
@@ -707,10 +716,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E82681EF-FAD9-45D1-B9CC-2256845934D0}">
-  <dimension ref="A1:CY2"/>
+  <dimension ref="A1:CY3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="AA2" sqref="AA2"/>
+    <sheetView tabSelected="1" topLeftCell="CO1" workbookViewId="0">
+      <selection activeCell="CZ3" sqref="CZ3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1409,6 +1418,317 @@
         <v>103</v>
       </c>
     </row>
+    <row r="3" spans="1:103" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E3" t="s">
+        <v>107</v>
+      </c>
+      <c r="F3" t="s">
+        <v>107</v>
+      </c>
+      <c r="G3" t="s">
+        <v>107</v>
+      </c>
+      <c r="H3" t="s">
+        <v>107</v>
+      </c>
+      <c r="I3" t="s">
+        <v>107</v>
+      </c>
+      <c r="J3" t="s">
+        <v>107</v>
+      </c>
+      <c r="K3" t="s">
+        <v>107</v>
+      </c>
+      <c r="L3" t="s">
+        <v>107</v>
+      </c>
+      <c r="M3" t="s">
+        <v>107</v>
+      </c>
+      <c r="N3" t="s">
+        <v>107</v>
+      </c>
+      <c r="O3" t="s">
+        <v>107</v>
+      </c>
+      <c r="P3" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>107</v>
+      </c>
+      <c r="R3" t="s">
+        <v>107</v>
+      </c>
+      <c r="S3" t="s">
+        <v>107</v>
+      </c>
+      <c r="T3" t="s">
+        <v>107</v>
+      </c>
+      <c r="U3" t="s">
+        <v>107</v>
+      </c>
+      <c r="V3" t="s">
+        <v>107</v>
+      </c>
+      <c r="W3" t="s">
+        <v>107</v>
+      </c>
+      <c r="X3" t="s">
+        <v>107</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>107</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>107</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>107</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>107</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>107</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>107</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>107</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>107</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>107</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>107</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>107</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>107</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>107</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>107</v>
+      </c>
+      <c r="AM3" t="s">
+        <v>107</v>
+      </c>
+      <c r="AN3" t="s">
+        <v>107</v>
+      </c>
+      <c r="AO3" t="s">
+        <v>107</v>
+      </c>
+      <c r="AP3" t="s">
+        <v>108</v>
+      </c>
+      <c r="AQ3" t="s">
+        <v>107</v>
+      </c>
+      <c r="AR3" t="s">
+        <v>107</v>
+      </c>
+      <c r="AS3" t="s">
+        <v>107</v>
+      </c>
+      <c r="AT3" t="s">
+        <v>107</v>
+      </c>
+      <c r="AU3" t="s">
+        <v>107</v>
+      </c>
+      <c r="AV3" t="s">
+        <v>107</v>
+      </c>
+      <c r="AW3" t="s">
+        <v>107</v>
+      </c>
+      <c r="AX3" t="s">
+        <v>107</v>
+      </c>
+      <c r="AY3" t="s">
+        <v>107</v>
+      </c>
+      <c r="AZ3" t="s">
+        <v>107</v>
+      </c>
+      <c r="BA3" t="s">
+        <v>107</v>
+      </c>
+      <c r="BB3" t="s">
+        <v>107</v>
+      </c>
+      <c r="BC3" t="s">
+        <v>107</v>
+      </c>
+      <c r="BD3" t="s">
+        <v>107</v>
+      </c>
+      <c r="BE3" t="s">
+        <v>107</v>
+      </c>
+      <c r="BF3" t="s">
+        <v>107</v>
+      </c>
+      <c r="BG3" t="s">
+        <v>107</v>
+      </c>
+      <c r="BH3" t="s">
+        <v>107</v>
+      </c>
+      <c r="BI3" t="s">
+        <v>107</v>
+      </c>
+      <c r="BJ3" t="s">
+        <v>107</v>
+      </c>
+      <c r="BK3" t="s">
+        <v>107</v>
+      </c>
+      <c r="BL3" t="s">
+        <v>107</v>
+      </c>
+      <c r="BM3" t="s">
+        <v>107</v>
+      </c>
+      <c r="BN3" t="s">
+        <v>107</v>
+      </c>
+      <c r="BO3" t="s">
+        <v>107</v>
+      </c>
+      <c r="BP3" t="s">
+        <v>107</v>
+      </c>
+      <c r="BQ3" t="s">
+        <v>107</v>
+      </c>
+      <c r="BR3" t="s">
+        <v>107</v>
+      </c>
+      <c r="BS3" t="s">
+        <v>107</v>
+      </c>
+      <c r="BT3" t="s">
+        <v>107</v>
+      </c>
+      <c r="BU3" t="s">
+        <v>107</v>
+      </c>
+      <c r="BV3" t="s">
+        <v>107</v>
+      </c>
+      <c r="BW3" t="s">
+        <v>107</v>
+      </c>
+      <c r="BX3" t="s">
+        <v>107</v>
+      </c>
+      <c r="BY3" t="s">
+        <v>107</v>
+      </c>
+      <c r="BZ3" t="s">
+        <v>107</v>
+      </c>
+      <c r="CA3" t="s">
+        <v>107</v>
+      </c>
+      <c r="CB3" t="s">
+        <v>107</v>
+      </c>
+      <c r="CC3" t="s">
+        <v>107</v>
+      </c>
+      <c r="CD3" t="s">
+        <v>107</v>
+      </c>
+      <c r="CE3" t="s">
+        <v>107</v>
+      </c>
+      <c r="CF3" t="s">
+        <v>107</v>
+      </c>
+      <c r="CG3" t="s">
+        <v>107</v>
+      </c>
+      <c r="CH3" t="s">
+        <v>107</v>
+      </c>
+      <c r="CI3" t="s">
+        <v>109</v>
+      </c>
+      <c r="CJ3" t="s">
+        <v>107</v>
+      </c>
+      <c r="CK3" t="s">
+        <v>107</v>
+      </c>
+      <c r="CL3" t="s">
+        <v>107</v>
+      </c>
+      <c r="CM3" t="s">
+        <v>107</v>
+      </c>
+      <c r="CN3" t="s">
+        <v>107</v>
+      </c>
+      <c r="CO3" t="s">
+        <v>107</v>
+      </c>
+      <c r="CP3" t="s">
+        <v>107</v>
+      </c>
+      <c r="CQ3" t="s">
+        <v>107</v>
+      </c>
+      <c r="CR3" t="s">
+        <v>107</v>
+      </c>
+      <c r="CS3" t="s">
+        <v>107</v>
+      </c>
+      <c r="CT3" t="s">
+        <v>107</v>
+      </c>
+      <c r="CU3" t="s">
+        <v>107</v>
+      </c>
+      <c r="CV3" t="s">
+        <v>107</v>
+      </c>
+      <c r="CW3" t="s">
+        <v>107</v>
+      </c>
+      <c r="CX3" t="s">
+        <v>107</v>
+      </c>
+      <c r="CY3" t="s">
+        <v>107</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>